<commit_message>
fix import with password&otority and create kurikulum with dropdown
</commit_message>
<xml_diff>
--- a/public/assets/excel/template.xlsx
+++ b/public/assets/excel/template.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>example@gmail.com</t>
   </si>
   <si>
     <t>Example_name</t>
+  </si>
+  <si>
+    <t>Example_password</t>
+  </si>
+  <si>
+    <t>Otoritas (Dosen/Penjamin Mutu)</t>
   </si>
 </sst>
 </file>
@@ -371,29 +377,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
   </sheetData>

</xml_diff>